<commit_message>
Normalized tables, added borders
</commit_message>
<xml_diff>
--- a/global results/globalSupersenseResults.xlsx
+++ b/global results/globalSupersenseResults.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan\Dizertatie\works\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dizertatie-bookNLP\global results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C917379-2B29-40A2-96E9-175516949B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6C5F57-1152-4CFC-9A20-8CA2DFF55FC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -480,14 +480,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection sqref="A1:D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -496,10 +496,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
         <v>42</v>
-      </c>
-      <c r="C1" t="s">
-        <v>43</v>
       </c>
       <c r="D1" t="s">
         <v>44</v>
@@ -510,10 +510,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C2" s="1">
         <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="C2" s="1">
-        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D2" s="1">
         <v>1.6999999999999999E-3</v>
@@ -524,10 +524,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
+        <v>3.3799999999999997E-2</v>
+      </c>
+      <c r="C3" s="1">
         <v>2.64E-2</v>
-      </c>
-      <c r="C3" s="1">
-        <v>3.3799999999999997E-2</v>
       </c>
       <c r="D3" s="1">
         <v>2.3300000000000001E-2</v>
@@ -538,10 +538,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="C4" s="1">
         <v>1.7600000000000001E-2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>1.3899999999999999E-2</v>
       </c>
       <c r="D4" s="1">
         <v>6.1000000000000004E-3</v>
@@ -552,10 +552,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
+        <v>9.2600000000000002E-2</v>
+      </c>
+      <c r="C5" s="1">
         <v>9.6500000000000002E-2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>9.2600000000000002E-2</v>
       </c>
       <c r="D5" s="1">
         <v>0.1482</v>
@@ -566,10 +566,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="C6" s="1">
         <v>1.6500000000000001E-2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>3.3000000000000002E-2</v>
       </c>
       <c r="D6" s="1">
         <v>1.89E-2</v>
@@ -580,10 +580,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
+        <v>1.54E-2</v>
+      </c>
+      <c r="C7" s="1">
         <v>2.9100000000000001E-2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>1.54E-2</v>
       </c>
       <c r="D7" s="1">
         <v>5.5399999999999998E-2</v>
@@ -594,10 +594,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
+        <v>4.2799999999999998E-2</v>
+      </c>
+      <c r="C8" s="1">
         <v>1.8700000000000001E-2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4.2799999999999998E-2</v>
       </c>
       <c r="D8" s="1">
         <v>1.7600000000000001E-2</v>
@@ -608,10 +608,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
+        <v>5.2900000000000003E-2</v>
+      </c>
+      <c r="C9" s="1">
         <v>4.2799999999999998E-2</v>
-      </c>
-      <c r="C9" s="1">
-        <v>5.2900000000000003E-2</v>
       </c>
       <c r="D9" s="1">
         <v>3.6900000000000002E-2</v>
@@ -622,10 +622,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="C10" s="1">
         <v>7.4000000000000003E-3</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1.4500000000000001E-2</v>
       </c>
       <c r="D10" s="1">
         <v>7.3000000000000001E-3</v>
@@ -636,10 +636,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
+        <v>1.29E-2</v>
+      </c>
+      <c r="C11" s="1">
         <v>7.6E-3</v>
-      </c>
-      <c r="C11" s="1">
-        <v>1.29E-2</v>
       </c>
       <c r="D11" s="1">
         <v>4.4000000000000003E-3</v>
@@ -650,10 +650,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="C12" s="1">
         <v>3.5000000000000001E-3</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2E-3</v>
       </c>
       <c r="D12" s="1">
         <v>4.1000000000000003E-3</v>
@@ -664,10 +664,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
+        <v>2.29E-2</v>
+      </c>
+      <c r="C13" s="1">
         <v>2.3E-2</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2.29E-2</v>
       </c>
       <c r="D13" s="1">
         <v>1.9699999999999999E-2</v>
@@ -678,10 +678,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
+        <v>6.5299999999999997E-2</v>
+      </c>
+      <c r="C14" s="1">
         <v>2.0299999999999999E-2</v>
-      </c>
-      <c r="C14" s="1">
-        <v>6.5299999999999997E-2</v>
       </c>
       <c r="D14" s="1">
         <v>4.3900000000000002E-2</v>
@@ -692,10 +692,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C15" s="1">
         <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="C15" s="1">
-        <v>8.0000000000000004E-4</v>
       </c>
       <c r="D15" s="1">
         <v>2.9999999999999997E-4</v>
@@ -706,10 +706,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
+        <v>3.7600000000000001E-2</v>
+      </c>
+      <c r="C16" s="1">
         <v>6.7999999999999996E-3</v>
-      </c>
-      <c r="C16" s="1">
-        <v>3.7600000000000001E-2</v>
       </c>
       <c r="D16" s="1">
         <v>1.03E-2</v>
@@ -720,10 +720,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
+        <v>6.9099999999999995E-2</v>
+      </c>
+      <c r="C17" s="1">
         <v>0.13089999999999999</v>
-      </c>
-      <c r="C17" s="1">
-        <v>6.9099999999999995E-2</v>
       </c>
       <c r="D17" s="1">
         <v>0.12189999999999999</v>
@@ -734,10 +734,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
+        <v>7.4000000000000003E-3</v>
+      </c>
+      <c r="C18" s="1">
         <v>2.8999999999999998E-3</v>
-      </c>
-      <c r="C18" s="1">
-        <v>7.4000000000000003E-3</v>
       </c>
       <c r="D18" s="1">
         <v>5.1999999999999998E-3</v>
@@ -748,10 +748,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="C19" s="1">
         <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="C19" s="1">
-        <v>5.1999999999999998E-3</v>
       </c>
       <c r="D19" s="1">
         <v>2.8999999999999998E-3</v>
@@ -762,10 +762,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="C20" s="1">
         <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1.6000000000000001E-3</v>
       </c>
       <c r="D20" s="1">
         <v>5.0000000000000001E-3</v>
@@ -776,10 +776,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="C21" s="1">
         <v>5.9999999999999995E-4</v>
-      </c>
-      <c r="C21" s="1">
-        <v>2.2000000000000001E-3</v>
       </c>
       <c r="D21" s="1">
         <v>1E-3</v>
@@ -790,10 +790,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
+        <v>1.11E-2</v>
+      </c>
+      <c r="C22" s="1">
         <v>7.1000000000000004E-3</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1.11E-2</v>
       </c>
       <c r="D22" s="1">
         <v>8.5000000000000006E-3</v>
@@ -804,10 +804,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
+        <v>3.8E-3</v>
+      </c>
+      <c r="C23" s="1">
         <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="C23" s="1">
-        <v>3.8E-3</v>
       </c>
       <c r="D23" s="1">
         <v>1.6999999999999999E-3</v>
@@ -818,10 +818,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="C24" s="1">
         <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="C24" s="1">
-        <v>3.5000000000000001E-3</v>
       </c>
       <c r="D24" s="1">
         <v>3.8E-3</v>
@@ -832,10 +832,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
+        <v>2.3599999999999999E-2</v>
+      </c>
+      <c r="C25" s="1">
         <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="C25" s="1">
-        <v>2.3599999999999999E-2</v>
       </c>
       <c r="D25" s="1">
         <v>1.24E-2</v>
@@ -846,10 +846,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
+        <v>2.0799999999999999E-2</v>
+      </c>
+      <c r="C26" s="1">
         <v>9.7999999999999997E-3</v>
-      </c>
-      <c r="C26" s="1">
-        <v>2.0799999999999999E-2</v>
       </c>
       <c r="D26" s="1">
         <v>3.2399999999999998E-2</v>
@@ -860,10 +860,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
+        <v>2.8899999999999999E-2</v>
+      </c>
+      <c r="C27" s="1">
         <v>2.3199999999999998E-2</v>
-      </c>
-      <c r="C27" s="1">
-        <v>2.8899999999999999E-2</v>
       </c>
       <c r="D27" s="1">
         <v>1.7899999999999999E-2</v>
@@ -874,10 +874,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
+        <v>4.3E-3</v>
+      </c>
+      <c r="C28" s="1">
         <v>1.0500000000000001E-2</v>
-      </c>
-      <c r="C28" s="1">
-        <v>4.3E-3</v>
       </c>
       <c r="D28" s="1">
         <v>1.3299999999999999E-2</v>
@@ -888,10 +888,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
+        <v>3.15E-2</v>
+      </c>
+      <c r="C29" s="1">
         <v>3.2899999999999999E-2</v>
-      </c>
-      <c r="C29" s="1">
-        <v>3.15E-2</v>
       </c>
       <c r="D29" s="1">
         <v>2.58E-2</v>
@@ -902,10 +902,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
+        <v>4.02E-2</v>
+      </c>
+      <c r="C30" s="1">
         <v>4.9599999999999998E-2</v>
-      </c>
-      <c r="C30" s="1">
-        <v>4.02E-2</v>
       </c>
       <c r="D30" s="1">
         <v>2.8299999999999999E-2</v>
@@ -916,10 +916,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
+        <v>4.82E-2</v>
+      </c>
+      <c r="C31" s="1">
         <v>9.4700000000000006E-2</v>
-      </c>
-      <c r="C31" s="1">
-        <v>4.82E-2</v>
       </c>
       <c r="D31" s="1">
         <v>5.1299999999999998E-2</v>
@@ -930,10 +930,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="C32" s="1">
         <v>2.7000000000000001E-3</v>
-      </c>
-      <c r="C32" s="1">
-        <v>1.6999999999999999E-3</v>
       </c>
       <c r="D32" s="1">
         <v>1.6000000000000001E-3</v>
@@ -944,10 +944,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="1">
+        <v>3.7000000000000002E-3</v>
+      </c>
+      <c r="C33" s="1">
         <v>5.1000000000000004E-3</v>
-      </c>
-      <c r="C33" s="1">
-        <v>3.7000000000000002E-3</v>
       </c>
       <c r="D33" s="1">
         <v>5.4999999999999997E-3</v>
@@ -958,10 +958,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="1">
+        <v>2.12E-2</v>
+      </c>
+      <c r="C34" s="1">
         <v>4.2599999999999999E-2</v>
-      </c>
-      <c r="C34" s="1">
-        <v>2.12E-2</v>
       </c>
       <c r="D34" s="1">
         <v>5.1200000000000002E-2</v>
@@ -972,10 +972,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="1">
+        <v>1.03E-2</v>
+      </c>
+      <c r="C35" s="1">
         <v>7.7000000000000002E-3</v>
-      </c>
-      <c r="C35" s="1">
-        <v>1.03E-2</v>
       </c>
       <c r="D35" s="1">
         <v>8.0000000000000002E-3</v>
@@ -986,10 +986,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
+        <v>1.15E-2</v>
+      </c>
+      <c r="C36" s="1">
         <v>1.35E-2</v>
-      </c>
-      <c r="C36" s="1">
-        <v>1.15E-2</v>
       </c>
       <c r="D36" s="1">
         <v>7.4999999999999997E-3</v>
@@ -1000,10 +1000,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
+        <v>3.9600000000000003E-2</v>
+      </c>
+      <c r="C37" s="1">
         <v>5.5100000000000003E-2</v>
-      </c>
-      <c r="C37" s="1">
-        <v>3.9600000000000003E-2</v>
       </c>
       <c r="D37" s="1">
         <v>5.8700000000000002E-2</v>
@@ -1014,10 +1014,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="1">
+        <v>3.56E-2</v>
+      </c>
+      <c r="C38" s="1">
         <v>3.5700000000000003E-2</v>
-      </c>
-      <c r="C38" s="1">
-        <v>3.56E-2</v>
       </c>
       <c r="D38" s="1">
         <v>3.3399999999999999E-2</v>
@@ -1028,10 +1028,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="1">
+        <v>1.55E-2</v>
+      </c>
+      <c r="C39" s="1">
         <v>2.92E-2</v>
-      </c>
-      <c r="C39" s="1">
-        <v>1.55E-2</v>
       </c>
       <c r="D39" s="1">
         <v>2.3199999999999998E-2</v>
@@ -1042,10 +1042,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="C40" s="1">
         <v>3.0599999999999999E-2</v>
-      </c>
-      <c r="C40" s="1">
-        <v>0.02</v>
       </c>
       <c r="D40" s="1">
         <v>1.8100000000000002E-2</v>
@@ -1056,10 +1056,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="1">
+        <v>9.0700000000000003E-2</v>
+      </c>
+      <c r="C41" s="1">
         <v>6.9199999999999998E-2</v>
-      </c>
-      <c r="C41" s="1">
-        <v>9.0700000000000003E-2</v>
       </c>
       <c r="D41" s="1">
         <v>6.1899999999999997E-2</v>
@@ -1070,10 +1070,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="1">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C42" s="1">
         <v>1E-4</v>
-      </c>
-      <c r="C42" s="1">
-        <v>2.0000000000000001E-4</v>
       </c>
       <c r="D42" s="1">
         <v>8.9999999999999998E-4</v>

</xml_diff>